<commit_message>
added 6 virtual tours
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/IC/Voodoo-Studio/Projects/Heraclee/Heraclee/resources/lang/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="37900" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="30580" yWindow="2920" windowWidth="33780" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="224">
   <si>
     <t>KEYS</t>
   </si>
@@ -679,19 +687,44 @@
   </si>
   <si>
     <t>Message send</t>
+  </si>
+  <si>
+    <t>ATTENTION!</t>
+  </si>
+  <si>
+    <t>Pay attention to all punctuation marks, Capital letters and spaces. Keep the same style as in the original please.</t>
+  </si>
+  <si>
+    <t>The original text is FRENCH (2nd column). Use it as model.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Pink</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> text do not touch. Modify only FR and EN columns if needed</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -730,6 +763,33 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="29"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -754,12 +814,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,14 +830,52 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1102,947 +1201,1119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C126"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="54.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54" style="3" customWidth="1"/>
+    <col min="2" max="2" width="64.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="54" style="6" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="20">
-      <c r="A4" s="1" t="s">
+    <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B9" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B10" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B11" s="12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B12" s="12" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B13" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B14" s="12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B15" s="12" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B18" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4" t="s">
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B19" s="12" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="4" t="s">
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B20" s="12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B21" s="12" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="4" t="s">
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B22" s="12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B23" s="12" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="4" t="s">
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="4" t="s">
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B25" s="12" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="4" t="s">
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B26" s="12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="4" t="s">
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="4" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B30" s="12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B31" s="12" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4" t="s">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="12" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B33" s="12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B34" s="12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="4" t="s">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B35" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="4" t="s">
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="12" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="4" t="s">
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B39" s="12" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="12" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="4" t="s">
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="12" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="4" t="s">
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="12" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="4" t="s">
+      <c r="C42" s="12"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="12" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="4" t="s">
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" s="12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B45" s="12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="4" t="s">
+      <c r="C45" s="12"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="12" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="12" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="4" t="s">
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B48" s="12" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="4" t="s">
+      <c r="C48" s="12"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B49" s="12" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="C49" s="12"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B50" s="12" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="4" t="s">
+      <c r="C50" s="12"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="12" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="4" t="s">
+      <c r="C51" s="12"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B52" s="12" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="4" t="s">
+      <c r="C52" s="12"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B53" s="12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="4" t="s">
+      <c r="C53" s="12"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B54" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="4" t="s">
+      <c r="C54" s="12"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B55" s="12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="4" t="s">
+      <c r="C55" s="12"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B56" s="12" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="4" t="s">
+      <c r="C56" s="12"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B57" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="4" t="s">
+      <c r="C57" s="12"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B58" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="4" t="s">
+      <c r="C58" s="12"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B59" s="12" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="4" t="s">
+      <c r="C59" s="12"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B60" s="12" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="4" t="s">
+      <c r="C60" s="12"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B61" s="12" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="4" t="s">
+      <c r="C61" s="12"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B62" s="12" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="4" t="s">
+      <c r="C62" s="12"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B63" s="12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="4" t="s">
+      <c r="C63" s="12"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B64" s="12" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="4" t="s">
+      <c r="C64" s="12"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B65" s="12" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="4" t="s">
+      <c r="C65" s="12"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B66" s="12" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="4" t="s">
+      <c r="C66" s="12"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B67" s="12" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="4" t="s">
+      <c r="C67" s="12"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B68" s="12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="4" t="s">
+      <c r="C68" s="12"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B69" s="12" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="4" t="s">
+      <c r="C69" s="12"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B70" s="12" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="4" t="s">
+      <c r="C70" s="12"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B71" s="12" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="4" t="s">
+      <c r="C71" s="12"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B72" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="4" t="s">
+      <c r="C72" s="12"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B73" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="4" t="s">
+      <c r="C73" s="12"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B74" s="12" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="4" t="s">
+      <c r="C74" s="12"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B75" s="12" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="4" t="s">
+      <c r="C75" s="12"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B76" s="12" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="4" t="s">
+      <c r="C76" s="12"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B77" s="12" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="4" t="s">
+      <c r="C77" s="12"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B78" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="4" t="s">
+      <c r="C78" s="12"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B79" s="12" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="4" t="s">
+      <c r="C79" s="12"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B80" s="12" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="4" t="s">
+      <c r="C80" s="12"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B81" s="12" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="4" t="s">
+      <c r="C81" s="12"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B82" s="12" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="4" t="s">
+      <c r="C82" s="12"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B83" s="12" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="4" t="s">
+      <c r="C83" s="12"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B84" s="12" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4" t="s">
+      <c r="C84" s="12"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B85" s="12" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="4" t="s">
+      <c r="C85" s="12"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B86" s="12" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="4" t="s">
+      <c r="C86" s="12"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B87" s="12" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="4" t="s">
+      <c r="C87" s="12"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B88" s="12" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="4" t="s">
+      <c r="C88" s="12"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B89" s="12" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="4" t="s">
+      <c r="C89" s="12"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B90" s="12" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="4" t="s">
+      <c r="C90" s="12"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B91" s="12" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="4" t="s">
+      <c r="C91" s="12"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B92" s="12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="4"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="4" t="s">
+      <c r="C92" s="12"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="4" t="s">
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
+    </row>
+    <row r="95" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B95" s="13" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="4" t="s">
+      <c r="C95" s="12"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B96" s="12" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="4" t="s">
+      <c r="C96" s="12"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B97" s="12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="4" t="s">
+      <c r="C97" s="12"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B98" s="12" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="4" t="s">
+      <c r="C98" s="12"/>
+    </row>
+    <row r="99" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B99" s="12" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="4"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="4" t="s">
+      <c r="C99" s="12"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="4" t="s">
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B102" s="12" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="4" t="s">
+      <c r="C102" s="12"/>
+    </row>
+    <row r="103" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B103" s="12" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="4" t="s">
+      <c r="C103" s="12"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B104" s="12" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="4"/>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="4" t="s">
+      <c r="C104" s="12"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="4" t="s">
+      <c r="B106" s="12"/>
+      <c r="C106" s="12"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B107" s="12" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="4" t="s">
+      <c r="C107" s="12"/>
+    </row>
+    <row r="108" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B108" s="12" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="4" t="s">
+      <c r="C108" s="12"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B109" s="12" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="4" t="s">
+      <c r="C109" s="12"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B110" s="12" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="4" t="s">
+      <c r="C110" s="12"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B111" s="12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="4" t="s">
+      <c r="C111" s="12"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B112" s="12" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="4" t="s">
+      <c r="C112" s="12"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B113" s="12" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="4" t="s">
+      <c r="C113" s="12"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B114" s="12" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="4" t="s">
+      <c r="C114" s="12"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B115" s="12" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="4" t="s">
+      <c r="C115" s="12"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B116" s="12" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="4" t="s">
+      <c r="C116" s="12"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B117" s="12" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="4" t="s">
+      <c r="C117" s="12"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B118" s="12" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="4" t="s">
+      <c r="C118" s="12"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B119" s="12" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="4"/>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="4" t="s">
+      <c r="C119" s="12"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="4" t="s">
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B122" s="12" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="4" t="s">
+      <c r="C122" s="12"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B123" s="12" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="4"/>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="4" t="s">
+      <c r="C123" s="12"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="4" t="s">
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B126" s="12" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="4" t="s">
+      <c r="C126" s="12"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B127" s="12" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="4" t="s">
+      <c r="C127" s="12"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B128" s="12" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="4" t="s">
+      <c r="C128" s="12"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B129" s="12" t="s">
         <v>219</v>
       </c>
+      <c r="C129" s="12"/>
     </row>
   </sheetData>
+  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tooltip on Fullscrin button, and fixed some small bugs on pagination and input number
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30580" yWindow="2920" windowWidth="33780" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="30420" yWindow="1100" windowWidth="33780" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="230">
   <si>
     <t>KEYS</t>
   </si>
@@ -713,6 +713,24 @@
       </rPr>
       <t xml:space="preserve"> text do not touch. Modify only FR and EN columns if needed</t>
     </r>
+  </si>
+  <si>
+    <t>Afficher l'image en plein écran</t>
+  </si>
+  <si>
+    <t>show_image_on_fullscreen</t>
+  </si>
+  <si>
+    <t>previous</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>Précédent</t>
+  </si>
+  <si>
+    <t>Suivant</t>
   </si>
 </sst>
 </file>
@@ -836,15 +854,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -861,6 +870,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1201,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1216,37 +1234,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1268,1045 +1286,1072 @@
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+        <v>227</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="12"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="12"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="12"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
+      <c r="A36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="12"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="12"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="12"/>
+        <v>225</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C45" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C48" s="12"/>
+        <v>42</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C49" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="9"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C51" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C55" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C57" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="9"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C58" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C59" s="12"/>
+        <v>53</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="9"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C60" s="12"/>
+        <v>54</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" s="12"/>
+        <v>55</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="9"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C62" s="12"/>
+        <v>56</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C63" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C65" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" s="9"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C67" s="12"/>
+        <v>61</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="9"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C68" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C70" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C72" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C73" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C75" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C76" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="C77" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="C78" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C79" s="12"/>
+        <v>73</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="C81" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C83" s="12"/>
+        <v>77</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C84" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C85" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C86" s="12"/>
+        <v>80</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C87" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C88" s="12"/>
+        <v>82</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C89" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C90" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C92" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
+      <c r="A93" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
-    </row>
-    <row r="95" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="9"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="C95" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C96" s="12"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+    </row>
+    <row r="98" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" s="9"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="9"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B97" s="12" t="s">
+      <c r="B100" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C97" s="12"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C98" s="12"/>
-    </row>
-    <row r="99" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B99" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C99" s="12"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="12"/>
-      <c r="C100" s="12"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="9"/>
+    </row>
+    <row r="102" spans="1:3" ht="38" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C102" s="12"/>
-    </row>
-    <row r="103" spans="1:3" ht="304" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C103" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C102" s="9"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="C104" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="12"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C105" s="9"/>
+    </row>
+    <row r="106" spans="1:3" ht="304" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B106" s="12"/>
-      <c r="C106" s="12"/>
+        <v>96</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B107" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C107" s="12"/>
-    </row>
-    <row r="108" spans="1:3" ht="304" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B108" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C108" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C107" s="9"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B109" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C109" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C110" s="12"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C110" s="9"/>
+    </row>
+    <row r="111" spans="1:3" ht="304" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="C111" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B112" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="C112" s="12"/>
+        <v>100</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C113" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C114" s="9"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C115" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B116" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="C116" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C117" s="12"/>
+        <v>105</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C118" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C119" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="12"/>
+      <c r="A120" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C122" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B123" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C123" s="12"/>
+      <c r="A123" s="4"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
+      <c r="A124" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B126" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C126" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B127" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="C127" s="12"/>
+      <c r="A127" s="4"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B128" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C128" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" s="9"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C130" s="9"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C131" s="9"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B132" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C129" s="12"/>
+      <c r="C132" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
Added DPE and GES translation and responsiveness on details page
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="256">
   <si>
     <t>KEYS</t>
   </si>
@@ -732,12 +732,109 @@
   <si>
     <t>Suivant</t>
   </si>
+  <si>
+    <t>energy_consumption_and_emission</t>
+  </si>
+  <si>
+    <t>energy_consumption</t>
+  </si>
+  <si>
+    <t>primary_energy_source</t>
+  </si>
+  <si>
+    <t>Consommation d’énergie et émissions</t>
+  </si>
+  <si>
+    <t>Consommation énergétique</t>
+  </si>
+  <si>
+    <t>(en énergie primaire)</t>
+  </si>
+  <si>
+    <t>energy_title_desc</t>
+  </si>
+  <si>
+    <r>
+      <t>pour le chauffage, la production d’eau chaude</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>&lt;br&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sanitaire et le refroidissement</t>
+    </r>
+  </si>
+  <si>
+    <t>conventional_energy_consumption</t>
+  </si>
+  <si>
+    <t>Consommation conventionnelle</t>
+  </si>
+  <si>
+    <t>energy_efficient_housing</t>
+  </si>
+  <si>
+    <t>Logement économe</t>
+  </si>
+  <si>
+    <t>high_energy_efficient_housing</t>
+  </si>
+  <si>
+    <t>Logement énergivore</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>Logement</t>
+  </si>
+  <si>
+    <t>emission_of_greenhouse_gases</t>
+  </si>
+  <si>
+    <t>Emission de gaz à effet de serre (GES)</t>
+  </si>
+  <si>
+    <t>emissions_estimate</t>
+  </si>
+  <si>
+    <t>Estimation des émissions :</t>
+  </si>
+  <si>
+    <t>low_greenhouse_gas_emissions</t>
+  </si>
+  <si>
+    <t>Faible émission de GES</t>
+  </si>
+  <si>
+    <t>high_greenhouse_gas_emissions</t>
+  </si>
+  <si>
+    <t>Forte émission de GES</t>
+  </si>
+  <si>
+    <t>year_short</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -807,6 +904,11 @@
       <sz val="14"/>
       <color theme="5" tint="0.39997558519241921"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1219,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2048,307 +2150,424 @@
       <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="9"/>
+      <c r="A96" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>233</v>
+      </c>
       <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B97" s="9"/>
+        <v>231</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>234</v>
+      </c>
       <c r="C97" s="9"/>
     </row>
-    <row r="98" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>195</v>
+        <v>232</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>235</v>
       </c>
       <c r="C98" s="9"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="38" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
       <c r="C99" s="9"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>93</v>
+        <v>240</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>198</v>
+        <v>241</v>
       </c>
       <c r="C101" s="9"/>
     </row>
-    <row r="102" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="C102" s="9"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="9"/>
+      <c r="A103" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>245</v>
+      </c>
       <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B104" s="9"/>
+        <v>246</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>247</v>
+      </c>
       <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>95</v>
+        <v>248</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>200</v>
+        <v>249</v>
       </c>
       <c r="C105" s="9"/>
     </row>
-    <row r="106" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>96</v>
+        <v>250</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>201</v>
+        <v>253</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="9"/>
+      <c r="A108" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>255</v>
+      </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A109" s="4"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>202</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B110" s="9"/>
       <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3" ht="304" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>203</v>
+        <v>90</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C114" s="9"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="38" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>208</v>
-      </c>
+      <c r="A116" s="4"/>
+      <c r="B116" s="9"/>
       <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>209</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B117" s="9"/>
       <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C118" s="9"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="304" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>213</v>
-      </c>
+      <c r="A121" s="4"/>
+      <c r="B121" s="9"/>
       <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>214</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B122" s="9"/>
       <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="9"/>
+      <c r="A123" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="C123" s="9"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="304" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B124" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="9"/>
+      <c r="A127" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B128" s="9"/>
+        <v>103</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>207</v>
+      </c>
       <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
       <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C131" s="9"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C132" s="9"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C133" s="9"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C134" s="9"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C135" s="9"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="4"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C138" s="9"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C139" s="9"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C142" s="9"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C143" s="9"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C144" s="9"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B132" s="9" t="s">
+      <c r="B145" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C132" s="9"/>
+      <c r="C145" s="9"/>
     </row>
   </sheetData>
   <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
footer text style modified
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="1100" windowWidth="33780" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="255">
   <si>
     <t>KEYS</t>
   </si>
@@ -335,33 +335,6 @@
     <t>copyright_text</t>
   </si>
   <si>
-    <t>footer_list_1</t>
-  </si>
-  <si>
-    <t>footer_list_2</t>
-  </si>
-  <si>
-    <t>footer_list_3</t>
-  </si>
-  <si>
-    <t>footer_list_4</t>
-  </si>
-  <si>
-    <t>footer_list_5</t>
-  </si>
-  <si>
-    <t>footer_list_6</t>
-  </si>
-  <si>
-    <t>footer_list_7</t>
-  </si>
-  <si>
-    <t>footer_list_8</t>
-  </si>
-  <si>
-    <t>footer_list_9</t>
-  </si>
-  <si>
     <t>email_title</t>
   </si>
   <si>
@@ -614,9 +587,6 @@
     <t>Informations</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum. Sed ut perspiciatis unde omnis iste natus error sit voluptatem accusantium doloremque laudantium, totam rem aperiam, eaque ipsa quae ab illo inventore veritatis et quasi architecto beatae vitae dicta sunt explicabo. Nemo enim ipsam voluptatem quia voluptas sit aspernatur aut odit aut fugit, sed quia consequuntur magni dolores eos qui ratione voluptatem sequi nesciunt. Neque porro quisquam est, qui dolorem ipsum quia dolor sit amet, consectetur, adipisci velit, sed quia non numquam eius modi tempora incidunt ut labore et dolore magnam aliquam quaerat voluptatem.</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
@@ -636,9 +606,6 @@
   </si>
   <si>
     <t>Heraclee - Agence Immobilière Saint Tropez</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum. Sed ut perspiciatis unde omnis iste natus error sit voluptatem accusantium doloremque laudantium, totam rem aperiam, eaque ipsa quae ab illo inventore veritatis et quasi architecto beatae vitae dicta sunt explicabo. Nemo enim ipsam voluptatem quia voluptas sit aspernatur aut odit aut fugit, sed quia consequuntur magni dolores eos qui ratione voluptatem sequi nesciunt. Neque porro quisquam est, qui dolorem ipsum quia dolor sit amet, consectetur, adipisci velit, sed quia non numquam eius modi tempora incidunt ut</t>
   </si>
   <si>
     <t>Inscrivez-vous à notre newsletter</t>
@@ -828,6 +795,38 @@
   </si>
   <si>
     <t>an</t>
+  </si>
+  <si>
+    <t>Notre agence Heraclee, spécialiste de l'immobilier de luxe au niveau de la Riviera Française, est basée depuis 7 ans dans l'emblématique ville de Saint Tropez. Le marché de l'immobilier de luxe de la Côte d'Azur étant l'un des plus attractif du pays, nous offrons à cet effet le meilleur de l'immobilier à St-Tropez. 
+De ce fait, en passant par les services de notre agence immobilière, les clients ont dès lors l'opportunité de pouvoir accéder à des biens d'exception via les nombreuses locations ou ventes situées pour la plupart dans les communes de St-Tropez et de Ramatuelle. De plus, l'immobilier de luxe s'avérant être en constante évolution tout comme les exigences et attentes de nos potentiels futurs acquéreurs, nous nous efforçons à ce titre de trouver le bien immobilier correspondant aux critères de sélection les plus pointus. 
+C'est d'ailleurs dans le but de garantir à notre clientèle une satisfaction totale que notre agence immobilière est composée d'une équipe d'experts disposant tous d'un large domaine de compétences, notamment en matière d'aspects juridiques et fiscaux. Le professionnalisme avéré de notre agence immobilière de St-Tropez, lui a entre autres permis de développer un réseau conséquent ayant lui-même conduit à la détention d'un portefeuille à fort potentiel.</t>
+  </si>
+  <si>
+    <t>footer_keyword_1</t>
+  </si>
+  <si>
+    <t>footer_keyword_2</t>
+  </si>
+  <si>
+    <t>footer_keyword_3</t>
+  </si>
+  <si>
+    <t>footer_keyword_4</t>
+  </si>
+  <si>
+    <t>footer_keyword_5</t>
+  </si>
+  <si>
+    <t>footer_keyword_6</t>
+  </si>
+  <si>
+    <t>footer_keyword_7</t>
+  </si>
+  <si>
+    <t>footer_keyword_8</t>
+  </si>
+  <si>
+    <t>footer_keyword_9</t>
   </si>
 </sst>
 </file>
@@ -911,7 +910,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -921,6 +920,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,7 +945,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,10 +971,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -981,6 +982,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1323,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1336,32 +1346,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1389,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C9" s="9"/>
     </row>
@@ -1398,7 +1408,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C10" s="9"/>
     </row>
@@ -1407,7 +1417,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C11" s="9"/>
     </row>
@@ -1416,7 +1426,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C12" s="9"/>
     </row>
@@ -1425,16 +1435,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C14" s="9"/>
     </row>
@@ -1443,25 +1453,25 @@
         <v>18</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C17" s="9"/>
     </row>
@@ -1482,7 +1492,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C20" s="9"/>
     </row>
@@ -1491,7 +1501,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C21" s="9"/>
     </row>
@@ -1500,7 +1510,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C22" s="9"/>
     </row>
@@ -1509,7 +1519,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C23" s="9"/>
     </row>
@@ -1518,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C24" s="9"/>
     </row>
@@ -1527,7 +1537,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C25" s="9"/>
     </row>
@@ -1536,7 +1546,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C26" s="9"/>
     </row>
@@ -1545,7 +1555,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C27" s="9"/>
     </row>
@@ -1554,7 +1564,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C28" s="9"/>
     </row>
@@ -1575,7 +1585,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C31" s="9"/>
     </row>
@@ -1584,7 +1594,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C32" s="9"/>
     </row>
@@ -1593,7 +1603,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C33" s="9"/>
     </row>
@@ -1602,7 +1612,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C34" s="9"/>
     </row>
@@ -1611,7 +1621,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C35" s="9"/>
     </row>
@@ -1620,7 +1630,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C36" s="9"/>
     </row>
@@ -1629,7 +1639,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C37" s="9"/>
     </row>
@@ -1650,7 +1660,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C40" s="9"/>
     </row>
@@ -1659,16 +1669,16 @@
         <v>36</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C42" s="9"/>
     </row>
@@ -1677,7 +1687,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C43" s="9"/>
     </row>
@@ -1686,7 +1696,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C44" s="9"/>
     </row>
@@ -1695,7 +1705,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C45" s="9"/>
     </row>
@@ -1704,7 +1714,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C46" s="9"/>
     </row>
@@ -1713,7 +1723,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C47" s="9"/>
     </row>
@@ -1722,7 +1732,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C48" s="9"/>
     </row>
@@ -1731,7 +1741,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C49" s="9"/>
     </row>
@@ -1740,7 +1750,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C50" s="9"/>
     </row>
@@ -1749,7 +1759,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C51" s="9"/>
     </row>
@@ -1758,7 +1768,7 @@
         <v>46</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C52" s="9"/>
     </row>
@@ -1767,7 +1777,7 @@
         <v>47</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C53" s="9"/>
     </row>
@@ -1776,7 +1786,7 @@
         <v>48</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C54" s="9"/>
     </row>
@@ -1785,7 +1795,7 @@
         <v>49</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C55" s="9"/>
     </row>
@@ -1794,7 +1804,7 @@
         <v>50</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C56" s="9"/>
     </row>
@@ -1803,7 +1813,7 @@
         <v>51</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C57" s="9"/>
     </row>
@@ -1812,7 +1822,7 @@
         <v>52</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C58" s="9"/>
     </row>
@@ -1821,7 +1831,7 @@
         <v>53</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C59" s="9"/>
     </row>
@@ -1830,7 +1840,7 @@
         <v>54</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C60" s="9"/>
     </row>
@@ -1839,7 +1849,7 @@
         <v>55</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C61" s="9"/>
     </row>
@@ -1848,7 +1858,7 @@
         <v>56</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C62" s="9"/>
     </row>
@@ -1857,7 +1867,7 @@
         <v>57</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C63" s="9"/>
     </row>
@@ -1866,7 +1876,7 @@
         <v>58</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C64" s="9"/>
     </row>
@@ -1875,7 +1885,7 @@
         <v>59</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C65" s="9"/>
     </row>
@@ -1884,7 +1894,7 @@
         <v>60</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C66" s="9"/>
     </row>
@@ -1893,7 +1903,7 @@
         <v>61</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C67" s="9"/>
     </row>
@@ -1902,7 +1912,7 @@
         <v>62</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C68" s="9"/>
     </row>
@@ -1911,7 +1921,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C69" s="9"/>
     </row>
@@ -1920,7 +1930,7 @@
         <v>64</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C70" s="9"/>
     </row>
@@ -1929,7 +1939,7 @@
         <v>65</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C71" s="9"/>
     </row>
@@ -1938,7 +1948,7 @@
         <v>66</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C72" s="9"/>
     </row>
@@ -1947,7 +1957,7 @@
         <v>67</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C73" s="9"/>
     </row>
@@ -1956,7 +1966,7 @@
         <v>68</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C74" s="9"/>
     </row>
@@ -1965,7 +1975,7 @@
         <v>69</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C75" s="9"/>
     </row>
@@ -1974,7 +1984,7 @@
         <v>70</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C76" s="9"/>
     </row>
@@ -1983,7 +1993,7 @@
         <v>71</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C77" s="9"/>
     </row>
@@ -1992,7 +2002,7 @@
         <v>72</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C78" s="9"/>
     </row>
@@ -2001,7 +2011,7 @@
         <v>73</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C79" s="9"/>
     </row>
@@ -2010,7 +2020,7 @@
         <v>74</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C80" s="9"/>
     </row>
@@ -2019,7 +2029,7 @@
         <v>75</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C81" s="9"/>
     </row>
@@ -2028,7 +2038,7 @@
         <v>76</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C82" s="9"/>
     </row>
@@ -2037,7 +2047,7 @@
         <v>77</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C83" s="9"/>
     </row>
@@ -2046,7 +2056,7 @@
         <v>78</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C84" s="9"/>
     </row>
@@ -2055,7 +2065,7 @@
         <v>79</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C85" s="9"/>
     </row>
@@ -2064,7 +2074,7 @@
         <v>80</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C86" s="9"/>
     </row>
@@ -2073,7 +2083,7 @@
         <v>81</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C87" s="9"/>
     </row>
@@ -2082,7 +2092,7 @@
         <v>82</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C88" s="9"/>
     </row>
@@ -2091,7 +2101,7 @@
         <v>83</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C89" s="9"/>
     </row>
@@ -2100,7 +2110,7 @@
         <v>84</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C90" s="9"/>
     </row>
@@ -2109,7 +2119,7 @@
         <v>85</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C91" s="9"/>
     </row>
@@ -2118,7 +2128,7 @@
         <v>86</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C92" s="9"/>
     </row>
@@ -2127,7 +2137,7 @@
         <v>87</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C93" s="9"/>
     </row>
@@ -2136,7 +2146,7 @@
         <v>88</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C94" s="9"/>
     </row>
@@ -2145,124 +2155,124 @@
         <v>89</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C97" s="9"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" ht="38" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C99" s="9"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C102" s="9"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C108" s="9"/>
     </row>
@@ -2278,13 +2288,11 @@
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
     </row>
-    <row r="111" spans="1:3" ht="304" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B111" s="10" t="s">
-        <v>195</v>
-      </c>
+      <c r="B111" s="16"/>
       <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2292,7 +2300,7 @@
         <v>91</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C112" s="9"/>
     </row>
@@ -2301,7 +2309,7 @@
         <v>92</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C113" s="9"/>
     </row>
@@ -2310,7 +2318,7 @@
         <v>93</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C114" s="9"/>
     </row>
@@ -2319,7 +2327,7 @@
         <v>94</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C115" s="9"/>
     </row>
@@ -2340,17 +2348,15 @@
         <v>95</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C118" s="9"/>
     </row>
-    <row r="119" spans="1:3" ht="304" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B119" s="9" t="s">
-        <v>195</v>
-      </c>
+      <c r="B119" s="15"/>
       <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2358,7 +2364,7 @@
         <v>97</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C120" s="9"/>
     </row>
@@ -2379,16 +2385,16 @@
         <v>98</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C123" s="9"/>
     </row>
-    <row r="124" spans="1:3" ht="304" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="409" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="C124" s="9"/>
     </row>
@@ -2397,7 +2403,7 @@
         <v>100</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C125" s="9"/>
     </row>
@@ -2406,88 +2412,88 @@
         <v>101</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>103</v>
+        <v>247</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>106</v>
+        <v>250</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C131" s="9"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C132" s="9"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>108</v>
+        <v>252</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C133" s="9"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>109</v>
+        <v>253</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C134" s="9"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C135" s="9"/>
     </row>
@@ -2505,19 +2511,19 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C138" s="9"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C139" s="9"/>
     </row>
@@ -2535,37 +2541,37 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C144" s="9"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C145" s="9"/>
     </row>

</xml_diff>

<commit_message>
news admin and edit modified
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -1459,11 +1459,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1524,14 +1526,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1872,7 +1876,7 @@
   <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3461,6 +3465,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
translations modified  masterfile for news
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="34620" yWindow="520" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="440">
   <si>
     <t>KEYS</t>
   </si>
@@ -1329,6 +1329,147 @@
   </si>
   <si>
     <t>I am interested</t>
+  </si>
+  <si>
+    <t>//NEWS PAGES</t>
+  </si>
+  <si>
+    <t>latest_news</t>
+  </si>
+  <si>
+    <t>Latest news</t>
+  </si>
+  <si>
+    <t>Dernières nouvelles</t>
+  </si>
+  <si>
+    <t>// AUTHORISATION</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>remember_me</t>
+  </si>
+  <si>
+    <t>log_in</t>
+  </si>
+  <si>
+    <t>list_of_articles</t>
+  </si>
+  <si>
+    <t>published</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>posting_date</t>
+  </si>
+  <si>
+    <t>article_text</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>publish</t>
+  </si>
+  <si>
+    <t>creating_article</t>
+  </si>
+  <si>
+    <t>editing_article</t>
+  </si>
+  <si>
+    <t>choose_header_img</t>
+  </si>
+  <si>
+    <t>choose_body_img</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>List of articles</t>
+  </si>
+  <si>
+    <t>Published</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Posting date</t>
+  </si>
+  <si>
+    <t>Article text</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>Creating new article</t>
+  </si>
+  <si>
+    <t>Editing article</t>
+  </si>
+  <si>
+    <t>Choose a header image</t>
+  </si>
+  <si>
+    <t>Choose a body image</t>
+  </si>
+  <si>
+    <t>Se souvenir de moi</t>
+  </si>
+  <si>
+    <t>Mot de passe</t>
+  </si>
+  <si>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Liste des articles</t>
+  </si>
+  <si>
+    <t>Publié</t>
+  </si>
+  <si>
+    <t>Titre</t>
+  </si>
+  <si>
+    <t>Date de publication</t>
+  </si>
+  <si>
+    <t>Texte de l'article</t>
+  </si>
+  <si>
+    <t>Enregistrer</t>
+  </si>
+  <si>
+    <t>Publier</t>
+  </si>
+  <si>
+    <t>Création d’article</t>
+  </si>
+  <si>
+    <t>Modification de l'article</t>
+  </si>
+  <si>
+    <t>Choisissez une image d'en-tête</t>
+  </si>
+  <si>
+    <t>Choisissez une image du corps</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C155"/>
+  <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3464,8 +3605,185 @@
         <v>386</v>
       </c>
     </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="16"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
TRanslation modified, added "no results found"
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="446">
   <si>
     <t>KEYS</t>
   </si>
@@ -1427,9 +1427,6 @@
     <t>Choose a header image</t>
   </si>
   <si>
-    <t>Choose a body image</t>
-  </si>
-  <si>
     <t>Se souvenir de moi</t>
   </si>
   <si>
@@ -1469,7 +1466,28 @@
     <t>Choisissez une image d'en-tête</t>
   </si>
   <si>
-    <t>Choisissez une image du corps</t>
+    <t>Choisissez une image ou pdf du corps</t>
+  </si>
+  <si>
+    <t>Choose a body image or pdf</t>
+  </si>
+  <si>
+    <t>currently_no_results</t>
+  </si>
+  <si>
+    <t>Actuellement aucune résultats</t>
+  </si>
+  <si>
+    <t>Currently no results found</t>
+  </si>
+  <si>
+    <t>currently_no_newsletters</t>
+  </si>
+  <si>
+    <t>Actuellement aucune newsletter</t>
+  </si>
+  <si>
+    <t>Currently no newsletters found</t>
   </si>
 </sst>
 </file>
@@ -2014,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2388,1402 +2406,1425 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="A39" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A40" s="7"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>281</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>198</v>
+        <v>36</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>197</v>
+        <v>131</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>138</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>289</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>392</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>141</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>290</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>144</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>292</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>149</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>296</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>157</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>323</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>368</v>
+        <v>165</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>308</v>
+        <v>166</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>172</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>312</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>175</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>313</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>183</v>
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>327</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>203</v>
+        <v>89</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B100" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C100" s="9" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
+    <row r="101" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B101" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C101" s="9" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B101" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>331</v>
+        <v>210</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="B106" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>371</v>
+        <v>217</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>334</v>
+        <v>219</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B110" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C110" s="9" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
-    </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A111" s="7"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="9"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>185</v>
-      </c>
+      <c r="B113" s="11"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>337</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B116" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C115" s="9" t="s">
+      <c r="C116" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="57" x14ac:dyDescent="0.25">
-      <c r="A116" s="7" t="s">
+    <row r="117" spans="1:3" ht="57" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B117" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C117" s="9" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
-      <c r="B117" s="9"/>
-      <c r="C117" s="9"/>
-    </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A118" s="7"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B120" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C119" s="9" t="s">
+      <c r="C120" s="9" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="10" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B120" s="12"/>
-      <c r="C120" s="9"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="7" t="s">
+      <c r="B121" s="12"/>
+      <c r="C121" s="9"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B122" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C122" s="9" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="9"/>
-      <c r="C122" s="9"/>
-    </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A123" s="7"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C125" s="9" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="409" x14ac:dyDescent="0.25">
-      <c r="A125" s="7" t="s">
+    <row r="126" spans="1:3" ht="409" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B125" s="9" t="s">
+      <c r="B126" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="C126" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B126" s="9" t="s">
+      <c r="B127" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C126" s="9" t="s">
+      <c r="C127" s="9" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
+    <row r="128" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="B128" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C127" s="9" t="s">
+      <c r="C128" s="9" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>250</v>
+        <v>231</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B134" s="9" t="s">
-        <v>251</v>
+        <v>232</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>250</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="B140" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="C139" s="9" t="s">
+      <c r="C140" s="9" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="7"/>
-      <c r="C140" s="9"/>
-    </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="7"/>
+      <c r="C141" s="9"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B141" s="9"/>
-      <c r="C141" s="9"/>
-    </row>
-    <row r="142" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A142" s="7" t="s">
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+    </row>
+    <row r="143" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A143" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B143" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C142" s="9" t="s">
+      <c r="C143" s="9" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="C143" s="9" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>374</v>
+        <v>103</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>378</v>
+        <v>238</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="B146" s="9" t="s">
+      <c r="B147" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="C146" s="9" t="s">
+      <c r="C147" s="9" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A147" s="7" t="s">
+    <row r="148" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A148" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B148" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C147" s="9" t="s">
+      <c r="C148" s="9" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="7"/>
-      <c r="B148" s="9"/>
-      <c r="C148" s="9"/>
-    </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A149" s="7"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B150" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>360</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B153" s="9" t="s">
+      <c r="B154" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="C153" s="9" t="s">
+      <c r="C154" s="9" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="B154" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="B155" s="8" t="s">
+      <c r="B156" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="C155" s="8" t="s">
+      <c r="C156" s="8" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="16"/>
-    </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="16" t="s">
-        <v>397</v>
-      </c>
+      <c r="A157" s="16"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="B158" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B159" s="8" t="s">
         <v>426</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="B160" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="C160" s="8" t="s">
+      <c r="B161" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C161" s="8" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="B174" s="8" t="s">
+      <c r="B175" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C175" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C174" s="8" t="s">
-        <v>425</v>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
gallery admin style fixed
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="486">
   <si>
     <t>KEYS</t>
   </si>
@@ -1599,6 +1599,15 @@
   </si>
   <si>
     <t>Check all images</t>
+  </si>
+  <si>
+    <t>choose_gallery_img</t>
+  </si>
+  <si>
+    <t>Choose image (min width 640px)</t>
+  </si>
+  <si>
+    <t>Choisir l'image (largeur min 640px)</t>
   </si>
 </sst>
 </file>
@@ -2143,10 +2152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A158" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -4065,66 +4074,77 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="16" t="s">
-        <v>461</v>
+        <v>483</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="16" t="s">
         <v>463</v>
       </c>
-      <c r="B192" s="8" t="s">
+      <c r="B193" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C192" s="8" t="s">
+      <c r="C193" s="8" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="16"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="16"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="16"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="16"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="16"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="16"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="16"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="16"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="16"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="16"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="16"/>
     </row>
   </sheetData>
   <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Added date of creation and updating date
</commit_message>
<xml_diff>
--- a/resources/lang/Masterfile_Heraclee.xlsx
+++ b/resources/lang/Masterfile_Heraclee.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="492">
   <si>
     <t>KEYS</t>
   </si>
@@ -1608,6 +1608,24 @@
   </si>
   <si>
     <t>Choisir l'image (largeur min 640px)</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>Created at:</t>
+  </si>
+  <si>
+    <t>Updated at:</t>
+  </si>
+  <si>
+    <t>Crée le :</t>
+  </si>
+  <si>
+    <t>Modifié le :</t>
   </si>
 </sst>
 </file>
@@ -2152,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120:XFD120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3352,772 +3370,780 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
-      <c r="B115" s="9"/>
-      <c r="C115" s="9"/>
+      <c r="A115" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B116" s="9"/>
-      <c r="C116" s="9"/>
+        <v>487</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B117" s="11"/>
+      <c r="A117" s="7"/>
+      <c r="B117" s="9"/>
       <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>337</v>
-      </c>
+      <c r="A119" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B119" s="11"/>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B121" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C121" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="57" x14ac:dyDescent="0.25">
-      <c r="A121" s="7" t="s">
+    <row r="122" spans="1:3" ht="57" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B122" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C122" s="9" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="9"/>
-      <c r="C122" s="9"/>
-    </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A123" s="7"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C125" s="9" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="10" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B125" s="12"/>
-      <c r="C125" s="9"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
+      <c r="B126" s="12"/>
+      <c r="C126" s="9"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B126" s="9" t="s">
+      <c r="B127" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C126" s="9" t="s">
+      <c r="C127" s="9" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="7"/>
-      <c r="B127" s="9"/>
-      <c r="C127" s="9"/>
-    </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A128" s="7"/>
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B129" s="9" t="s">
+      <c r="B130" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C129" s="9" t="s">
+      <c r="C130" s="9" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="409" x14ac:dyDescent="0.25">
-      <c r="A130" s="7" t="s">
+    <row r="131" spans="1:3" ht="409" x14ac:dyDescent="0.25">
+      <c r="A131" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B130" s="9" t="s">
+      <c r="B131" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="C130" s="9" t="s">
+      <c r="C131" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="7" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B132" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C131" s="9" t="s">
+      <c r="C132" s="9" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A132" s="7" t="s">
+    <row r="133" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A133" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B132" s="9" t="s">
+      <c r="B133" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C132" s="9" t="s">
+      <c r="C133" s="9" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C133" s="9" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>250</v>
+        <v>231</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>251</v>
+        <v>232</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>250</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B144" s="9" t="s">
+      <c r="B145" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="C144" s="9" t="s">
+      <c r="C145" s="9" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="7"/>
-      <c r="C145" s="9"/>
-    </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="7" t="s">
+      <c r="A146" s="7"/>
+      <c r="C146" s="9"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B146" s="9"/>
-      <c r="C146" s="9"/>
-    </row>
-    <row r="147" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A147" s="7" t="s">
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+    </row>
+    <row r="148" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A148" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B148" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C147" s="9" t="s">
+      <c r="C148" s="9" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="C148" s="9" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>374</v>
+        <v>103</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>378</v>
+        <v>238</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="B151" s="9" t="s">
+      <c r="B152" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="C151" s="9" t="s">
+      <c r="C152" s="9" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="38" x14ac:dyDescent="0.25">
-      <c r="A152" s="7" t="s">
+    <row r="153" spans="1:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="A153" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B153" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C152" s="9" t="s">
+      <c r="C153" s="9" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="7"/>
-      <c r="B153" s="9"/>
-      <c r="C153" s="9"/>
-    </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A154" s="7"/>
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>360</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B158" s="9" t="s">
+      <c r="B159" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="C158" s="9" t="s">
+      <c r="C159" s="9" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="C159" s="8" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="B160" s="8" t="s">
+      <c r="B161" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="C160" s="8" t="s">
+      <c r="C161" s="8" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="16"/>
-    </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
-        <v>397</v>
-      </c>
+      <c r="A162" s="16"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="B165" s="8" t="s">
+      <c r="B166" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C166" s="8" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="16" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="C168" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="16" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="16" t="s">
-        <v>443</v>
+        <v>411</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="16" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>475</v>
+        <v>445</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>455</v>
       </c>
-      <c r="B182" s="8" t="s">
+      <c r="B183" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="C182" s="8" t="s">
+      <c r="C183" s="8" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="16"/>
-    </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
-        <v>466</v>
-      </c>
+      <c r="A184" s="16"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="16" t="s">
-        <v>456</v>
-      </c>
-      <c r="B185" s="8" t="s">
-        <v>467</v>
-      </c>
-      <c r="C185" s="8" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="16" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="16" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="16" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="16" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="16" t="s">
-        <v>461</v>
+        <v>483</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="16" t="s">
         <v>463</v>
       </c>
-      <c r="B193" s="8" t="s">
+      <c r="B194" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C193" s="8" t="s">
+      <c r="C194" s="8" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="16"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="16"/>
@@ -4145,6 +4171,9 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="16"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="16"/>
     </row>
   </sheetData>
   <sheetProtection password="9488" sheet="1" objects="1" scenarios="1"/>

</xml_diff>